<commit_message>
update repnonsive comment slide, file task
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NMH\Desktop\BC51_CAPSTONE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\BC51_CAPSTONE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4A6708-7E75-4668-B9A4-E276F3EEF518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -114,16 +115,22 @@
   </si>
   <si>
     <t>hoang</t>
+  </si>
+  <si>
+    <t>son</t>
+  </si>
+  <si>
+    <t>backtotop chua hoan thien</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +161,24 @@
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -309,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -335,9 +360,6 @@
     <xf numFmtId="164" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -348,18 +370,32 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,30 +634,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:E12"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="14.25" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="13.8" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="4" width="7.625" customWidth="1"/>
-    <col min="5" max="5" width="10.25" customWidth="1"/>
-    <col min="6" max="6" width="7.625" customWidth="1"/>
-    <col min="7" max="7" width="9.25" customWidth="1"/>
-    <col min="8" max="8" width="7.625" customWidth="1"/>
-    <col min="9" max="9" width="8.75" customWidth="1"/>
+    <col min="2" max="4" width="7.59765625" customWidth="1"/>
+    <col min="5" max="5" width="10.19921875" customWidth="1"/>
+    <col min="6" max="6" width="7.59765625" customWidth="1"/>
+    <col min="7" max="7" width="9.19921875" customWidth="1"/>
+    <col min="8" max="8" width="7.59765625" customWidth="1"/>
+    <col min="9" max="9" width="8.69921875" customWidth="1"/>
     <col min="10" max="10" width="33" customWidth="1"/>
-    <col min="11" max="26" width="7.625" customWidth="1"/>
+    <col min="11" max="26" width="7.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,242 +689,355 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="12">
-        <v>0.8</v>
-      </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="13" t="s">
+      <c r="B2" s="14">
+        <v>45061</v>
+      </c>
+      <c r="C2" s="14">
+        <v>45062</v>
+      </c>
+      <c r="D2" s="15">
+        <v>1</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="20">
+        <v>45062</v>
+      </c>
+      <c r="G2" s="20">
+        <v>45063</v>
+      </c>
+      <c r="H2" s="15">
+        <v>1</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="13"/>
-    </row>
-    <row r="4" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="14">
+        <v>45061</v>
+      </c>
+      <c r="C3" s="14">
+        <v>45062</v>
+      </c>
+      <c r="D3" s="15">
+        <v>1</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="20">
+        <v>45063</v>
+      </c>
+      <c r="G3" s="20">
+        <v>45064</v>
+      </c>
+      <c r="H3" s="15">
+        <v>1</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="13"/>
-    </row>
-    <row r="5" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="B4" s="14">
+        <v>45063</v>
+      </c>
+      <c r="C4" s="14">
+        <v>45064</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="20">
+        <v>45064</v>
+      </c>
+      <c r="G4" s="20">
+        <v>45065</v>
+      </c>
+      <c r="H4" s="15">
+        <v>1</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="13"/>
-    </row>
-    <row r="6" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="B5" s="14">
+        <v>45065</v>
+      </c>
+      <c r="C5" s="18">
+        <v>45066</v>
+      </c>
+      <c r="D5" s="15">
+        <v>1</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="20">
+        <v>45066</v>
+      </c>
+      <c r="G5" s="20">
+        <v>45067</v>
+      </c>
+      <c r="H5" s="15">
+        <v>1</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="B6" s="14">
+        <v>45067</v>
+      </c>
+      <c r="C6" s="18">
+        <v>45069</v>
+      </c>
+      <c r="D6" s="15">
+        <v>1</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="20">
+        <v>45069</v>
+      </c>
+      <c r="G6" s="20">
+        <v>45070</v>
+      </c>
+      <c r="H6" s="15">
+        <v>1</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="17"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="14">
+        <v>45070</v>
+      </c>
+      <c r="C7" s="18">
+        <v>45070</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="20">
+        <v>45070</v>
+      </c>
+      <c r="G7" s="20">
+        <v>45071</v>
+      </c>
+      <c r="H7" s="15">
+        <v>1</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="13"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="10">
-        <v>1</v>
-      </c>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F8" s="20">
+        <v>45064</v>
+      </c>
+      <c r="G8" s="20">
+        <v>45064</v>
+      </c>
+      <c r="H8" s="15">
+        <v>1</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="10">
-        <v>1</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="13"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F9" s="20">
+        <v>45066</v>
+      </c>
+      <c r="G9" s="20">
+        <v>45066</v>
+      </c>
+      <c r="H9" s="15">
+        <v>1</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="11" t="s">
+      <c r="C10" s="14">
+        <v>45074</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F10" s="20">
+        <v>45074</v>
+      </c>
+      <c r="G10" s="20">
+        <v>45072</v>
+      </c>
+      <c r="H10" s="15">
+        <v>1</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="10">
-        <v>1</v>
-      </c>
-      <c r="E11" s="11" t="s">
+      <c r="D11" s="15">
+        <v>1</v>
+      </c>
+      <c r="E11" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="13"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F11" s="14">
+        <v>45073</v>
+      </c>
+      <c r="G11" s="14">
+        <v>45073</v>
+      </c>
+      <c r="H11" s="15">
+        <v>1</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="10">
-        <v>1</v>
-      </c>
-      <c r="E12" s="11" t="s">
+      <c r="D12" s="15">
+        <v>1</v>
+      </c>
+      <c r="E12" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F12" s="14">
+        <v>45073</v>
+      </c>
+      <c r="G12" s="14">
+        <v>45073</v>
+      </c>
+      <c r="H12" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="13"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="13"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="12"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="D2:D14">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2 H4:H14">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="H2:H14">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>